<commit_message>
Corrigiendo nombres de columnas
</commit_message>
<xml_diff>
--- a/Datos/Bases JASP/Binomiales_Wins.xlsx
+++ b/Datos/Bases JASP/Binomiales_Wins.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Periodo</t>
   </si>
@@ -98,10 +98,13 @@
     <t>Right 4</t>
   </si>
   <si>
-    <t>Right 1</t>
+    <t>1+O:O</t>
   </si>
   <si>
-    <t>1+O:O</t>
+    <t>Right1_2</t>
+  </si>
+  <si>
+    <t>Right 2</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
   <dimension ref="A1:Z77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,10 +523,10 @@
         <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L1" t="s">
         <v>21</v>
@@ -1608,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="Z14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrigiendo bases porque no se habia quitado la sesion 3
</commit_message>
<xml_diff>
--- a/Datos/Bases JASP/Binomiales_Wins.xlsx
+++ b/Datos/Bases JASP/Binomiales_Wins.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Jaime_Lab25\Datos\Bases JASP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Jaime_Lab25\Datos\Bases JASP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -551,7 +551,7 @@
   <dimension ref="A1:AP115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AM6" sqref="AM6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,22 +559,20 @@
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="15" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="8.140625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="7.85546875" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="27" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="28" max="33" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="10" max="15" width="11.42578125" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" customWidth="1"/>
+    <col min="19" max="19" width="8.140625" customWidth="1"/>
+    <col min="20" max="20" width="7.85546875" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" customWidth="1"/>
+    <col min="23" max="33" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Agregando tirada Low por cada periodo para cada una de las sesiones corridas
</commit_message>
<xml_diff>
--- a/Datos/Bases JASP/Binomiales_Wins.xlsx
+++ b/Datos/Bases JASP/Binomiales_Wins.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Jaime_Lab25\Datos\Bases JASP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Jaime_Lab25\Datos\Bases JASP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Periodo</t>
   </si>
@@ -151,6 +151,42 @@
   <si>
     <t>W_Periodo8</t>
   </si>
+  <si>
+    <t>Pre_Periodo1</t>
+  </si>
+  <si>
+    <t>Pre_Periodo2</t>
+  </si>
+  <si>
+    <t>Pre_Periodo3</t>
+  </si>
+  <si>
+    <t>Pre_Periodo4</t>
+  </si>
+  <si>
+    <t>L_Periodo1</t>
+  </si>
+  <si>
+    <t>L_Periodo2</t>
+  </si>
+  <si>
+    <t>L_Periodo3</t>
+  </si>
+  <si>
+    <t>L_Periodo4</t>
+  </si>
+  <si>
+    <t>L_Periodo5</t>
+  </si>
+  <si>
+    <t>L_Periodo6</t>
+  </si>
+  <si>
+    <t>L_Periodo7</t>
+  </si>
+  <si>
+    <t>L_Periodo8</t>
+  </si>
 </sst>
 </file>
 
@@ -174,7 +210,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +277,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -254,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -268,6 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP115"/>
+  <dimension ref="A1:BB115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="AT17" sqref="AT17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,22 +603,24 @@
     <col min="2" max="2" width="8.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="15" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" customWidth="1"/>
-    <col min="19" max="19" width="8.140625" customWidth="1"/>
-    <col min="20" max="20" width="7.85546875" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" customWidth="1"/>
-    <col min="23" max="33" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="10" max="15" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="8.140625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="7.85546875" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" hidden="1" customWidth="1"/>
+    <col min="23" max="33" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="35" max="42" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="43" max="46" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -702,8 +747,44 @@
       <c r="AP1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -716,7 +797,7 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="13">
         <v>0</v>
       </c>
       <c r="F2" s="2">
@@ -785,10 +866,10 @@
       <c r="AA2">
         <v>0</v>
       </c>
-      <c r="AB2" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="7">
+      <c r="AB2" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="13">
         <v>1</v>
       </c>
       <c r="AD2" s="9">
@@ -830,8 +911,44 @@
       <c r="AP2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>1</v>
+      </c>
+      <c r="AS2">
+        <v>1</v>
+      </c>
+      <c r="AT2">
+        <v>1</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>1</v>
+      </c>
+      <c r="AY2">
+        <v>1</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>1</v>
+      </c>
+      <c r="BB2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -844,7 +961,7 @@
       <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="13">
         <v>1</v>
       </c>
       <c r="F3" s="2">
@@ -913,10 +1030,10 @@
       <c r="AA3">
         <v>1</v>
       </c>
-      <c r="AB3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="7">
+      <c r="AB3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="13">
         <v>0</v>
       </c>
       <c r="AD3" s="9">
@@ -958,8 +1075,44 @@
       <c r="AP3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ3">
+        <v>1</v>
+      </c>
+      <c r="AR3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>1</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>1</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>1</v>
+      </c>
+      <c r="AZ3">
+        <v>0</v>
+      </c>
+      <c r="BA3">
+        <v>0</v>
+      </c>
+      <c r="BB3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -972,7 +1125,7 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="13">
         <v>1</v>
       </c>
       <c r="F4" s="2">
@@ -1041,10 +1194,10 @@
       <c r="AA4">
         <v>1</v>
       </c>
-      <c r="AB4" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="7">
+      <c r="AB4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="13">
         <v>1</v>
       </c>
       <c r="AD4" s="9">
@@ -1086,8 +1239,44 @@
       <c r="AP4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>1</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>1</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4">
+        <v>0</v>
+      </c>
+      <c r="BA4">
+        <v>1</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1100,7 +1289,7 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="13">
         <v>1</v>
       </c>
       <c r="F5" s="2">
@@ -1169,10 +1358,10 @@
       <c r="AA5">
         <v>6</v>
       </c>
-      <c r="AB5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="7">
+      <c r="AB5" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="13">
         <v>1</v>
       </c>
       <c r="AD5" s="9">
@@ -1214,8 +1403,44 @@
       <c r="AP5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ5">
+        <v>1</v>
+      </c>
+      <c r="AR5">
+        <v>1</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>1</v>
+      </c>
+      <c r="AU5">
+        <v>1</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
+      <c r="AX5">
+        <v>1</v>
+      </c>
+      <c r="AY5">
+        <v>1</v>
+      </c>
+      <c r="AZ5">
+        <v>1</v>
+      </c>
+      <c r="BA5">
+        <v>0</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1228,7 +1453,7 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="13">
         <v>1</v>
       </c>
       <c r="F6" s="2">
@@ -1297,10 +1522,10 @@
       <c r="AA6">
         <v>1</v>
       </c>
-      <c r="AB6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="7">
+      <c r="AB6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="13">
         <v>1</v>
       </c>
       <c r="AD6" s="9">
@@ -1342,8 +1567,44 @@
       <c r="AP6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ6">
+        <v>1</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>1</v>
+      </c>
+      <c r="AU6">
+        <v>1</v>
+      </c>
+      <c r="AV6">
+        <v>1</v>
+      </c>
+      <c r="AW6">
+        <v>1</v>
+      </c>
+      <c r="AX6">
+        <v>1</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
+      </c>
+      <c r="AZ6">
+        <v>0</v>
+      </c>
+      <c r="BA6">
+        <v>1</v>
+      </c>
+      <c r="BB6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1356,7 +1617,7 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="13">
         <v>1</v>
       </c>
       <c r="F7" s="2">
@@ -1425,10 +1686,10 @@
       <c r="AA7">
         <v>0</v>
       </c>
-      <c r="AB7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="7">
+      <c r="AB7" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="13">
         <v>0</v>
       </c>
       <c r="AD7" s="9">
@@ -1470,8 +1731,44 @@
       <c r="AP7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ7">
+        <v>1</v>
+      </c>
+      <c r="AR7">
+        <v>1</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>1</v>
+      </c>
+      <c r="AU7">
+        <v>1</v>
+      </c>
+      <c r="AV7">
+        <v>1</v>
+      </c>
+      <c r="AW7">
+        <v>1</v>
+      </c>
+      <c r="AX7">
+        <v>1</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
+      </c>
+      <c r="AZ7">
+        <v>0</v>
+      </c>
+      <c r="BA7">
+        <v>0</v>
+      </c>
+      <c r="BB7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1484,7 +1781,7 @@
       <c r="D8" s="1">
         <v>0</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="13">
         <v>0</v>
       </c>
       <c r="F8" s="2">
@@ -1553,10 +1850,10 @@
       <c r="AA8">
         <v>6</v>
       </c>
-      <c r="AB8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="7">
+      <c r="AB8" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="13">
         <v>0</v>
       </c>
       <c r="AD8" s="9">
@@ -1598,8 +1895,44 @@
       <c r="AP8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ8">
+        <v>1</v>
+      </c>
+      <c r="AR8">
+        <v>1</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>1</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8">
+        <v>0</v>
+      </c>
+      <c r="AX8">
+        <v>1</v>
+      </c>
+      <c r="AY8">
+        <v>0</v>
+      </c>
+      <c r="AZ8">
+        <v>1</v>
+      </c>
+      <c r="BA8">
+        <v>0</v>
+      </c>
+      <c r="BB8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1612,7 +1945,7 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="13">
         <v>1</v>
       </c>
       <c r="F9" s="2">
@@ -1681,10 +2014,10 @@
       <c r="AA9">
         <v>1</v>
       </c>
-      <c r="AB9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="7">
+      <c r="AB9" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="13">
         <v>1</v>
       </c>
       <c r="AD9" s="9">
@@ -1726,8 +2059,44 @@
       <c r="AP9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>1</v>
+      </c>
+      <c r="AS9">
+        <v>1</v>
+      </c>
+      <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9">
+        <v>1</v>
+      </c>
+      <c r="AW9">
+        <v>1</v>
+      </c>
+      <c r="AX9">
+        <v>1</v>
+      </c>
+      <c r="AY9">
+        <v>0</v>
+      </c>
+      <c r="AZ9">
+        <v>1</v>
+      </c>
+      <c r="BA9">
+        <v>1</v>
+      </c>
+      <c r="BB9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1740,7 +2109,7 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="13">
         <v>0</v>
       </c>
       <c r="F10" s="2">
@@ -1809,10 +2178,10 @@
       <c r="AA10">
         <v>0</v>
       </c>
-      <c r="AB10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="7">
+      <c r="AB10" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="13">
         <v>0</v>
       </c>
       <c r="AD10" s="9">
@@ -1854,8 +2223,44 @@
       <c r="AP10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ10">
+        <v>1</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>1</v>
+      </c>
+      <c r="AT10">
+        <v>1</v>
+      </c>
+      <c r="AU10">
+        <v>0</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10">
+        <v>1</v>
+      </c>
+      <c r="AX10">
+        <v>1</v>
+      </c>
+      <c r="AY10">
+        <v>0</v>
+      </c>
+      <c r="AZ10">
+        <v>0</v>
+      </c>
+      <c r="BA10">
+        <v>0</v>
+      </c>
+      <c r="BB10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1868,7 +2273,7 @@
       <c r="D11" s="1">
         <v>0</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="13">
         <v>0</v>
       </c>
       <c r="F11" s="2">
@@ -1937,10 +2342,10 @@
       <c r="AA11">
         <v>6</v>
       </c>
-      <c r="AB11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="7">
+      <c r="AB11" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="13">
         <v>0</v>
       </c>
       <c r="AD11" s="9">
@@ -1982,8 +2387,44 @@
       <c r="AP11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>1</v>
+      </c>
+      <c r="AS11">
+        <v>1</v>
+      </c>
+      <c r="AT11">
+        <v>1</v>
+      </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AV11">
+        <v>1</v>
+      </c>
+      <c r="AW11">
+        <v>0</v>
+      </c>
+      <c r="AX11">
+        <v>1</v>
+      </c>
+      <c r="AY11">
+        <v>0</v>
+      </c>
+      <c r="AZ11">
+        <v>1</v>
+      </c>
+      <c r="BA11">
+        <v>0</v>
+      </c>
+      <c r="BB11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1996,7 +2437,7 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="13">
         <v>1</v>
       </c>
       <c r="F12" s="2">
@@ -2065,10 +2506,10 @@
       <c r="AA12">
         <v>1</v>
       </c>
-      <c r="AB12" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="7">
+      <c r="AB12" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="13">
         <v>1</v>
       </c>
       <c r="AD12" s="9">
@@ -2084,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -2097,7 +2538,7 @@
       <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="13">
         <v>0</v>
       </c>
       <c r="F13" s="2">
@@ -2166,10 +2607,10 @@
       <c r="AA13">
         <v>1</v>
       </c>
-      <c r="AB13" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="7">
+      <c r="AB13" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="13">
         <v>0</v>
       </c>
       <c r="AD13" s="9">
@@ -2185,7 +2626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -2198,7 +2639,7 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="13">
         <v>1</v>
       </c>
       <c r="F14" s="2">
@@ -2267,10 +2708,10 @@
       <c r="AA14">
         <v>1</v>
       </c>
-      <c r="AB14" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC14" s="7">
+      <c r="AB14" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="13">
         <v>1</v>
       </c>
       <c r="AD14" s="9">
@@ -2286,7 +2727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -2299,7 +2740,7 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="13">
         <v>1</v>
       </c>
       <c r="F15" s="2">
@@ -2368,10 +2809,10 @@
       <c r="AA15">
         <v>1</v>
       </c>
-      <c r="AB15" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="7">
+      <c r="AB15" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="13">
         <v>1</v>
       </c>
       <c r="AD15" s="9">
@@ -2387,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -2400,7 +2841,7 @@
       <c r="D16" s="1">
         <v>0</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="13">
         <v>0</v>
       </c>
       <c r="F16" s="2">
@@ -2469,10 +2910,10 @@
       <c r="AA16">
         <v>8</v>
       </c>
-      <c r="AB16" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="7">
+      <c r="AB16" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="13">
         <v>0</v>
       </c>
       <c r="AD16" s="9">
@@ -2501,7 +2942,7 @@
       <c r="D17" s="1">
         <v>0</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="13">
         <v>1</v>
       </c>
       <c r="F17" s="2">
@@ -2570,10 +3011,10 @@
       <c r="AA17">
         <v>7</v>
       </c>
-      <c r="AB17" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC17" s="7">
+      <c r="AB17" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="13">
         <v>0</v>
       </c>
       <c r="AD17" s="9">
@@ -2602,7 +3043,7 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="13">
         <v>1</v>
       </c>
       <c r="F18" s="2">
@@ -2671,10 +3112,10 @@
       <c r="AA18">
         <v>0</v>
       </c>
-      <c r="AB18" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC18" s="7">
+      <c r="AB18" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="13">
         <v>0</v>
       </c>
       <c r="AD18" s="9">
@@ -2703,7 +3144,7 @@
       <c r="D19" s="1">
         <v>1</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="13">
         <v>0</v>
       </c>
       <c r="F19" s="2">
@@ -2772,10 +3213,10 @@
       <c r="AA19">
         <v>1</v>
       </c>
-      <c r="AB19" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC19" s="7">
+      <c r="AB19" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="13">
         <v>0</v>
       </c>
       <c r="AD19" s="9">
@@ -2804,7 +3245,7 @@
       <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="13">
         <v>0</v>
       </c>
       <c r="F20" s="2">
@@ -2873,10 +3314,10 @@
       <c r="AA20">
         <v>1</v>
       </c>
-      <c r="AB20" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC20" s="7">
+      <c r="AB20" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="13">
         <v>1</v>
       </c>
       <c r="AD20" s="9">
@@ -2905,7 +3346,7 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="13">
         <v>1</v>
       </c>
       <c r="F21" s="2">
@@ -2974,10 +3415,10 @@
       <c r="AA21">
         <v>1</v>
       </c>
-      <c r="AB21" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC21" s="7">
+      <c r="AB21" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="13">
         <v>1</v>
       </c>
       <c r="AD21" s="9">
@@ -3006,7 +3447,7 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="13">
         <v>1</v>
       </c>
       <c r="F22" s="2">
@@ -3075,10 +3516,10 @@
       <c r="AA22">
         <v>1</v>
       </c>
-      <c r="AB22" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC22" s="7">
+      <c r="AB22" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="13">
         <v>0</v>
       </c>
       <c r="AD22" s="9">
@@ -3107,7 +3548,7 @@
       <c r="D23" s="1">
         <v>0</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="13">
         <v>1</v>
       </c>
       <c r="F23" s="2">
@@ -3176,10 +3617,10 @@
       <c r="AA23">
         <v>6</v>
       </c>
-      <c r="AB23" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC23" s="7">
+      <c r="AB23" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC23" s="13">
         <v>0</v>
       </c>
       <c r="AD23" s="9">
@@ -3208,7 +3649,7 @@
       <c r="D24" s="1">
         <v>0</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="13">
         <v>0</v>
       </c>
       <c r="F24" s="2">
@@ -3277,10 +3718,10 @@
       <c r="AA24">
         <v>0</v>
       </c>
-      <c r="AB24" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC24" s="7">
+      <c r="AB24" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="13">
         <v>0</v>
       </c>
       <c r="AD24" s="9">
@@ -3309,7 +3750,7 @@
       <c r="D25" s="1">
         <v>1</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="13">
         <v>1</v>
       </c>
       <c r="F25" s="2">
@@ -3378,10 +3819,10 @@
       <c r="AA25">
         <v>1</v>
       </c>
-      <c r="AB25" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC25" s="7">
+      <c r="AB25" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="13">
         <v>0</v>
       </c>
       <c r="AD25" s="9">
@@ -3410,7 +3851,7 @@
       <c r="D26" s="1">
         <v>0</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="13">
         <v>1</v>
       </c>
       <c r="F26" s="2">
@@ -3479,10 +3920,10 @@
       <c r="AA26">
         <v>7</v>
       </c>
-      <c r="AB26" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC26" s="7">
+      <c r="AB26" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="13">
         <v>0</v>
       </c>
       <c r="AD26" s="9">
@@ -3511,7 +3952,7 @@
       <c r="D27" s="1">
         <v>1</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="13">
         <v>1</v>
       </c>
       <c r="F27" s="2">
@@ -3580,10 +4021,10 @@
       <c r="AA27">
         <v>1</v>
       </c>
-      <c r="AB27" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="7">
+      <c r="AB27" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="13">
         <v>1</v>
       </c>
       <c r="AD27" s="9">
@@ -3612,7 +4053,7 @@
       <c r="D28" s="1">
         <v>0</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="13">
         <v>0</v>
       </c>
       <c r="F28" s="2">
@@ -3681,10 +4122,10 @@
       <c r="AA28">
         <v>1</v>
       </c>
-      <c r="AB28" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="7">
+      <c r="AB28" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="13">
         <v>0</v>
       </c>
       <c r="AD28" s="9">
@@ -3713,7 +4154,7 @@
       <c r="D29" s="1">
         <v>0</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="13">
         <v>0</v>
       </c>
       <c r="F29" s="2">
@@ -3782,10 +4223,10 @@
       <c r="AA29">
         <v>0</v>
       </c>
-      <c r="AB29" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC29" s="7">
+      <c r="AB29" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC29" s="13">
         <v>0</v>
       </c>
       <c r="AD29" s="9">
@@ -3883,10 +4324,10 @@
       <c r="AA30">
         <v>7</v>
       </c>
-      <c r="AB30" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC30" s="7">
+      <c r="AB30" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="13">
         <v>0</v>
       </c>
       <c r="AD30" s="9">
@@ -3984,10 +4425,10 @@
       <c r="AA31">
         <v>2</v>
       </c>
-      <c r="AB31" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC31" s="7">
+      <c r="AB31" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC31" s="13">
         <v>1</v>
       </c>
       <c r="AD31" s="9">
@@ -4085,10 +4526,10 @@
       <c r="AA32">
         <v>1</v>
       </c>
-      <c r="AB32" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC32" s="7">
+      <c r="AB32" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC32" s="13">
         <v>1</v>
       </c>
       <c r="AD32" s="9">
@@ -4186,10 +4627,10 @@
       <c r="AA33">
         <v>1</v>
       </c>
-      <c r="AB33" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC33" s="7">
+      <c r="AB33" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC33" s="13">
         <v>0</v>
       </c>
       <c r="AD33" s="9">
@@ -4290,7 +4731,7 @@
       <c r="AB34" s="7">
         <v>0</v>
       </c>
-      <c r="AC34" s="7">
+      <c r="AC34" s="13">
         <v>0</v>
       </c>
       <c r="AD34" s="9">
@@ -4391,7 +4832,7 @@
       <c r="AB35" s="7">
         <v>0</v>
       </c>
-      <c r="AC35" s="7">
+      <c r="AC35" s="13">
         <v>0</v>
       </c>
       <c r="AD35" s="9">
@@ -4492,7 +4933,7 @@
       <c r="AB36" s="7">
         <v>1</v>
       </c>
-      <c r="AC36" s="7">
+      <c r="AC36" s="13">
         <v>0</v>
       </c>
       <c r="AD36" s="9">
@@ -4593,7 +5034,7 @@
       <c r="AB37" s="7">
         <v>1</v>
       </c>
-      <c r="AC37" s="7">
+      <c r="AC37" s="13">
         <v>1</v>
       </c>
       <c r="AD37" s="9">

</xml_diff>